<commit_message>
updated feature completion for map generation
</commit_message>
<xml_diff>
--- a/Hashi/hashi_features.xlsx
+++ b/Hashi/hashi_features.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xfill\Documents\SP21_ATLS4320_MobileAppDev\atls4320_mobileappdev\Hashi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574C1393-AA9A-4104-9077-7982F36E7BD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F09D2EB-C0EA-4152-8223-5A7BD640AE8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{8CF6AAC1-059C-4AEB-9435-81827B7D19B5}"/>
   </bookViews>
@@ -335,7 +335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,12 +378,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -397,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -405,7 +399,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -729,8 +722,8 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="218" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +841,7 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C7">
@@ -882,7 +875,7 @@
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C9">
@@ -950,7 +943,7 @@
       <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C13">
@@ -1001,7 +994,7 @@
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -1018,7 +1011,7 @@
       <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C17">
@@ -1035,7 +1028,7 @@
       <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C18">

</xml_diff>